<commit_message>
changes made- no writing on excel files
</commit_message>
<xml_diff>
--- a/keywords0.xlsx
+++ b/keywords0.xlsx
@@ -453,15 +453,15 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>tarazzo tiles</t>
+          <t>tarazzo tiles for home</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>8100</v>
+        <v>0</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>tarazzo tiles</t>
+          <t>tarazzo tiles for home</t>
         </is>
       </c>
     </row>

</xml_diff>